<commit_message>
Revert "Revert "Daylight Saving2""
This reverts commit 5e435b83fe0963285760dbbaba79ececa6a531e6.
</commit_message>
<xml_diff>
--- a/Daylight Saving Time.xlsx
+++ b/Daylight Saving Time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
     <t>Year</t>
   </si>
@@ -726,10 +726,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,6 +879,147 @@
         <v>November 5</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f>"March"&amp;" "&amp;ROUNDUP(14-MOD((1+A14*5/4),7),0)</f>
+        <v>March 9</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>"November"&amp;" "&amp;ROUNDUP(7-MOD((1+A14*5/4),7),0)</f>
+        <v>November 2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f t="shared" ref="B15:B23" si="2">"March"&amp;" "&amp;ROUNDUP(14-MOD((1+A15*5/4),7),0)</f>
+        <v>March 8</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f t="shared" ref="C15:C23" si="3">"November"&amp;" "&amp;ROUNDUP(7-MOD((1+A15*5/4),7),0)</f>
+        <v>November 1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>March 13</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>November 6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>March 12</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>November 5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>March 11</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>November 4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>March 10</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>November 3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>March 8</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>November 1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>March 14</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>November 7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>March 13</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>November 6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>March 12</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>November 5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>